<commit_message>
Updating SPMP and others
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Project\EduCycle_Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3030D48D-2F82-453B-B757-EEA4A5985F69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37514C8-C473-47C9-BCB8-DC1466779BBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67875" yWindow="7605" windowWidth="29820" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="64320" yWindow="10440" windowWidth="31680" windowHeight="17205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -252,7 +252,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.25277406674876546"/>
-          <c:y val="6.4861579358056767E-2"/>
+          <c:y val="5.3481778504571711E-2"/>
           <c:w val="0.73054574339345024"/>
           <c:h val="0.93513842064194319"/>
         </c:manualLayout>
@@ -1397,16 +1397,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>60324</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3105150</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>577850</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>60324</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1734,7 +1734,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>